<commit_message>
- incompatible change Workbook::parse_range API, now returns a list of [$book, $sheet, $row, $col, $range] - add Workbook::_rowcol_to_range() - add tests for Workbook::names and Workbook::parse_range - add Cell::formula() and Cell::get_hyperlink()
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/link01.xlsx
+++ b/t/regression/xlsx_files/link01.xlsx
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="NAMED">Sheet1!$C$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -69,6 +69,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>string</t>
@@ -109,6 +110,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -147,7 +149,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,24 +447,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="str">
+        <f>HYPERLINK("[link01.xlsx]Sheet1!A5","ByFormula")</f>
+        <v>ByFormula</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="str">
+        <f>HYPERLINK("[link01.xlsx]A5","ByFormula2")</f>
+        <v>ByFormula2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -473,13 +484,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>5+5</f>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -487,7 +498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
@@ -510,7 +521,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -527,7 +538,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -565,7 +576,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>